<commit_message>
Actualización de gráfico estudiantes
</commit_message>
<xml_diff>
--- a/data/ld_7.xlsx
+++ b/data/ld_7.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pirm/Downloads/ld-dashboard-main/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pirm/Desktop/usaer_dashboard-main/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C6A1103-FD80-B44C-8B0B-9A539A29496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F287B392-F51C-7C4F-87BB-9D7B90152FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="680" windowWidth="27640" windowHeight="16940" xr2:uid="{C46359CF-482B-0F41-926D-D871A68F524C}"/>
+    <workbookView xWindow="9320" yWindow="500" windowWidth="27640" windowHeight="16040" xr2:uid="{C46359CF-482B-0F41-926D-D871A68F524C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921596E1-A5F5-654B-9058-2E6CD3A7F095}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,8 +473,9 @@
       <c r="C2" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -485,7 +486,7 @@
         <v>8085</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -496,7 +497,7 @@
         <v>64337</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -507,7 +508,7 @@
         <v>20315</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -518,7 +519,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -529,7 +530,7 @@
         <v>61828</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -540,7 +541,7 @@
         <v>269711</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -551,7 +552,7 @@
         <v>51874</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -562,7 +563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -573,7 +574,7 @@
         <v>5414</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -584,7 +585,7 @@
         <v>16608</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -595,7 +596,7 @@
         <v>3743</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -606,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -617,7 +618,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>

</xml_diff>